<commit_message>
adding some more pdfs
</commit_message>
<xml_diff>
--- a/OperatingSystem/OperatingSystemConceptsHighLevelChart.xlsx
+++ b/OperatingSystem/OperatingSystemConceptsHighLevelChart.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20295" windowHeight="8445"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20295" windowHeight="8445" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t>Computer-System Operation</t>
   </si>
@@ -495,12 +495,1267 @@
     <t>Sumary:
 Don’t forgot to read entire Summary concept…</t>
   </si>
+  <si>
+    <t>In this chapter we are exploring on vantage of following OS aspects.
+* Services OS provides to users, processes and other systems
+* Interfaces available to users and programmers
+* OS components and their interconnections.</t>
+  </si>
+  <si>
+    <t>OS Services</t>
+  </si>
+  <si>
+    <t>User and OS Interface</t>
+  </si>
+  <si>
+    <t>Command-line Interface or Command Interpreters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Here entered commands to be performed by OS.
+* Some OS treat this Command Interpreter as part of kernel and some are as special program.
+* On OS where Command interpreters are choosen from available multiple list is to be called "shell" e.g. Bourne shell, Bourne-again shellh, korn shell, cshell etc...
+* Commands given in this level includes manupalating files like, deleting, creating, editing, list, print, copy and execute...
+* These command can be implemented in two ways...
+a) command interpreter containes code to executes given command.
+b) Executing command using OS Programs, here Command interpreter doesn't understand given command any way; it merely uses the comand to identify a file to be loaded into memory to execute given command.
+e.g. In UNIX to delete file...rm file.txt here would search for a file called rm, load the file into memory, and execute it with the parameter file.txt. The function associated with the rm command would be defined completely by the code in the file rm.
+</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>Some examples for open source graphical inteface environment are KDE and GNOME for Linix and Unix OS.
+And Some examples for Commercial version of UNIX are "Common Desktop Environment" (CDE) and X-Windows Systems</t>
+  </si>
+  <si>
+    <t>Choice of Interface</t>
+  </si>
+  <si>
+    <t>* Sys Admins and Power Users uses command line interpretors.
+* It typically is substantially removed from the actual system structure. The design of a useful and friendly user interface is therefore not a direct function of the operating system.</t>
+  </si>
+  <si>
+    <t>System Calls</t>
+  </si>
+  <si>
+    <t>* simple programs may make heavy use of the operating system. Frequently, systems execute thousands of system calls per second.
+* A programmer accesses an API via a library of code provided by the operating system.
+* Each operating system has its own name for each system call.
+* Behind the scenes, the functions that make up an API typically invoke the actual system calls on behalf of the application programmer.
+* Why would an application programmer prefer programming according to an API rather than invoking actual system calls? There are several reasons for doing so. One benefit concerns program portability. An application programmer designing a program using an API can expect her program to compile and run on any system that supports the same API.
+Furthermore, actual system calls can often be more detailed and difficult to work with than the API available to an application programmer. Nevertheless, there often exists a strong correlation between a function in the API and its associated system call within the kernel. In fact, many of the POSIX and Windows APIs are similar to the native system calls provided by the UNIX, Linux, and Windows operating systems.
+* For most programming languages, the run-time support system (a set of functions built into libraries included with a compiler) provides a systemcall interface that serves as the link to system calls made available by the operating system. The system-call interface intercepts function calls in the API and invokes the necessary system calls within the operating system. Typically, a number is associated with each system call, and the system-call interface maintains a table indexed according to these numbers. The system call interface then invokes the intended system call in the operating-system kernel and returns the status of the system call and any return values. most of the details of the operating-system interface are hidden from the programmer by the API and are managed by the run-time support library.
+* Three general methods are used to pass parameters to OS.
+-&gt; The simplest approach is to pass the parameters in registers.
+-&gt;  In some cases, however, there may be more parameters than registers. In these cases, the parameters are generally stored in a block, or table, in memory, and the address of the block is passed as a parameter in a register. This is the approach taken by Linux and Solaris. -&gt; Parameters also can be placed, or pushed, onto the stack by the program and popped off the stack by the operating system.</t>
+  </si>
+  <si>
+    <t>* OS provides certain services to programs and to the users of those programs.
+* Following are the functions provided by OS Services to Users.
+A) User Interface: Command Line Interface (CLI), Batch Interface and GUI.
+B) Program Execution:
+C) I/O Operations: 
+* For specific devices, special functions may be desired in OS to accomplish I/O operations during program execution.
+* For efficiency and protection, users usually cannot control I/O devices directly. Therefore, the operating system must provide a means to do I/O.
+D) File-System Manipulation:
+* Here OS include permissions management to allow or deny access to files or directories based on file ownership.
+E) Communications:
+* Here one process needs to exchange information with another process.
+Such communication may occur between processes that are executing on the same computer or between processes that are executing on different computer systems tied together by a computer network.
+* Communications implemented via...
+a) Shared Memory: Here two more processes read and write shared section of memory.
+b) Message Passing: here predined format information packets are moved between processes by OS.
+F) Error detection: 
+* The program must be able to end its execution, either normally or abnormally (indicating error). Hence OS needs to be detecting and correcting errors constantly. these errors may occur in...
+1) CPU and Memory hardware(such as memory eror and power failure)
+2) In I/O devices (such as parity error on disk, a network connection failure...)
+3) In the user program (such as an airthmetic overflow, illigal memory location access or too greate use of CPU time).
+* For each type of error, the OS should take the appropriate action
+to ensure correct and consistent computing. like...
+1) Sometimes, it has no choice but to halt the system. 
+2) At other times, it might terminate an error-causing
+process
+3) or return an error code to a process for the process to detect and
+possibly correct.
+* Following are the functions provided by OS Services to ensure efficient operation of system itself.
+A) Resource Allocation:
+The OS manages many different types of resources. 
+Some (such as CPU cycles, main memory, and file storage) may have special allocation code. For instance, in determining how best to use
+the CPU, operating systems have CPU-scheduling routines that take into
+account the speed of the CPU, the jobs that must be executed, the number of registers available, and other factors., whereas others (such as I/O devices) may have much more general request and release code. e.g. Theremay also be routines to allocate printers, USB storage drives, and other peripheral devices.
+B) Accounting: 
+We want to keep track of which users use how much and what kinds of computer resources.
+C) Protection and Security:
+When owners of information stored in a multiuser or networked computer system may want to control use of that information. Hence Protection involves ensuring that all access to system resources is controlled. And through Security we can authenticate users to access system resources by means of login features.</t>
+  </si>
+  <si>
+    <t>Types of System Calls.
+They are grouped roughly into 6 major categories</t>
+  </si>
+  <si>
+    <t>Process Control:
+* end and abort
+* load and execute
+* create and terminate process
+* get process attributes and set process attributes
+* wait for time
+* wait event, signal event
+* allocate and free memory</t>
+  </si>
+  <si>
+    <r>
+      <t>* A running program needs to be able to halt its execution either normally (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>end()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) or abnormally (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>abort()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">).
+* A process or job executing one program may want to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">load() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">and
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>execute()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> another program.
+* An interesting question is where to return control when the loaded program terminates. This question is related to whether the existing program is lost, saved, or allowed to continue execution concurrently
+with the new program.
+* If control returns to the existing program when the new program terminates, we must save the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>memory image of the existing program</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; thus, we have effectively created a mechanism for one program to call another program. If both programs continue concurrently, we have created a new job or process to be multiprogrammed. Often, there is a system call specifically for this purpose (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>create process() or submit job()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>).
+* Control of newly created process execution is done by</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> get process attributes() and set process attributes() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">for setting job's priority, its max allowable execution time... 
+* And terminate the process or job using </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">terminate_process() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">call.
+* Also use </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">wait_time(), wait_event() and signal_event() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">sys calls to control process or job executions.
+* Quite often, two or more processes may share data. To ensure the integrity of the data being shared, operating systems often provide system calls allowing a process to lock shared data. Then, no other process can access the data until the lock is released. Typically, such system calls include acquire </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lock()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>release_lock()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+ * An examples for variations in process and job control 
+a) Single-tasking system: MS-DOS OS
+b) Mutitasking-System: FreeBSD OS (uses </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fork(), exec(), exit()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sys calls).</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">File Manipulation/Management:
+* Create and Delete file
+* open and close file
+* read, write and reposition file
+* get file attributes and set file attributes
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* File operations can be done using </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>carete(), delete(), open(), read(), write(), reposition() and close()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Sys calls.
+* File attributes include the file name, file type, protection codes, accounting information, and so on. At least two system calls, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>get file attributes() and set file attributes()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, are required for this function.
+* Some OS provide many more calls, such as calls for file </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>move()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>copy()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Device Manipulation/Management:
+* Request and Release device
+* read, write and reposition
+* get device attributes and set device attributes
+* logically attach or detach devices</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* A process may need several resources to execute—main memory, disk drives, access to files, and so on.
+* The various resources controlled by the OS can be thought of as devices. Some of these devices are physical devices (for example, disk
+drives), while others can be thought of as abstract or virtual devices (for
+example, files).
+* Asystem with multiple users may require us to first </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>request()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> a device, to ensure exclusive use of it. After we are finished with the device, we
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>release()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> it.
+* Once the device has been requested (and allocated to us), we can </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>read(), write()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and (possibly) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>reposition()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the device, just as we can with files.
+*The user interface can also make files and devices appear to be similar, even though the underlying system calls are dissimilar. This is another example of the many design decisions that go into building an operating system and user interface.</t>
+    </r>
+  </si>
+  <si>
+    <t>Information Maintenance:
+* Get time or date, set time or date.
+* get system data and set system data.
+* get process, file, or device attributes.
+* set process, file, or device attributes.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* Many system calls exist simply for the purpose of transferring information between the user program and the operating system. E.g. current </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>time(), date()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Other system calls may return information about the system, such as the number of current users, the version number of the operating system, the amount of free memory or disk space, and so on.
+* Another set of system calls is helpful in debugging a program. Many
+systems provide system calls to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dump()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> memory. This provision is useful for debugging. A program trace lists each system call as it is executed.
+* Even microprocessors provide a CPU mode known as single step, in which a trap is executed by the CPU after every instruction. The trap is usually caught by a debugger.
+* Many OS provide a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>time profile of a program</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to indicate the amount of time that the program executes at a particular location or set of locations. A time profile requires either a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tracing facility</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>regular timer
+interrupts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. At every occurrence of the timer interrupt, the value of the program counter is recorded. With sufficiently frequent timer interrupts, a statistical picture of the time spent on various parts of the program can be obtained.
+* Generally, calls are also used to reset the process information (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>get process attributes()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>set process attributes()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <t>Communications:
+* create, delete communication connection
+* send, receive messages
+* trasfer status information
+* attatch or detach remote devices.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* There are two common models of interprocess communication: the message passing model and the shared-memory model.
+A) Message-Passing Model:
+-&gt; Messages can be exchanged between the processes either directly
+or indirectly through a common mailbox.
+-&gt; Before communication can take place, a connection must be opened. The name of the other communicator must be known, be it another process on the same system or a process on another computer connected by a communications network. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>host name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> has </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>network identifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> such as IP address. Similarly, each process has a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>process
+name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and this name is translated into an identifier by which the operating system can refer to the process. The </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>get hostid()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>get processid()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> system calls do this translation. The identifiers are then passed to the general purpose </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>open()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>close()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> calls provided by the file system or to specific </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>open connection()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>close connection()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> system calls, depending on the system’s model of communication. The recipient process usually must give its permission for communication to take place with an accept </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>connection()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> call.
+-&gt; Most processes that will be receiving connections are </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>special-purpose
+daemons</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,which are system programs provided for that purpose. They execute a wait for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>connection()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> call and are awakened when a connection is made.
+-&gt; The source of the communication, known as the</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> client</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and the receiving daemon, knownas a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>server</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, then exchange messages by using read </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>message()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and write </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>message()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> system calls.
+-&gt; The close </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>connection()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> call terminates the communication.
+-&gt; It is useful for exchanging smaller amounts of data, because no conflicts need be avoided. It is also easier to implement than is shared memory for intercomputer communication.
+B) Shared-Memory Model:
+-&gt; In the shared-memory model, processes use </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>shared_memory_create()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>shared_memory_attach()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> system calls to create and gain access to regions of memory owned by other processes.
+-&gt; Recall that, normally, the operating system tries to prevent one process from accessing another process’s memory. Shared memory requires that two or more processes agree to remove this restriction. They can then exchange information by reading and writing data in the shared areas.
+-&gt; The form of the data is determined by the processes and is not under the operating system’s control. The processes are also responsible for
+ensuring that they are not writing to the same location simultaneously.
+-&gt; It allows maximum speed and convenience of communication, since it
+can be done at memory transfer speeds when it takes place within a computer.
+-&gt; Problems exist, however, in the areas of protection and synchronization between the processes sharing memory.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Protection:
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">* Protection provides a mechanism for controlling access to the resources provided by a computer system.
+* Typically, system calls providing protection include </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>set_permission()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>get_permission()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, which manipulate the permission settings of
+resources such as files and disks. The </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>allow_user()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>deny_user()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> system calls specify whether particular users can—or cannot—be allowed access to certain resources.</t>
+    </r>
+  </si>
+  <si>
+    <t>System Programs</t>
+  </si>
+  <si>
+    <t>* System Programs are also known as "Sytesm Utilities" which provides convenient environment for program development and execution. Some of them are simply user interfaces to system calls. 
+* Following are categories of System Programs.
+A) File management: 
+These programs create, delete, copy, rename, print, dump, list, and generally manipulate files and directories.
+B) Status Information:
+-&gt; Some programs simply ask the system for the date, time, amount of available memory or disk space, number of users, or similar status information.
+-&gt; Others are more complex, providing detailed performance, logging, and debugging information. Typically, these programs format and print the output to the terminal or other output devices or files or display it in a window of the GUI.
+-&gt; Some systems also support a registry, which is used to store and retrieve configuration information.
+C) File Modification:
+There may also be special commands to search contents of files or perform transformations of the text.
+D) Programming-language support:
+Compilers, assemblers, debuggers, and interpreters for common programming languages (such as C, C++, Java, and PERL) are often provided with the operating system or available as a separate download.
+E) Program loading and execution:
+The OS may provide absolute loaders, relocatable loaders, linkage editors, and overlay loaders. Debugging systems for either higher-level languages or machine language are needed as well.
+F) Communications:
+These programs provide the mechanism for creating virtual connections among processes, users, and computer systems. They allow users to send messages to one another’s screens, to browse Web pages, to send e-mail messages, to log in remotely, or to transfer files from one machine to another.
+G) Background Services:
+-&gt; All general-purpose systems have methods for launching certain system-program processes at boot time. Some of these processes terminate after completing their tasks, while others continue to run until the system is halted.
+-&gt; Constantly running system-program processes are known as services, subsystems, or daemons.
+e.g. 
+* A system needed a service to listen for network connections in order to connect those requests to the correct processes.
+* Other examples include process schedulers that start processes according to a specified schedule
+* system error monitoring services
+* and print servers.
+-&gt; In addition, operating systems that run important activities in user context rather than in kernel context may use daemons to run these
+activities.</t>
+  </si>
+  <si>
+    <t>Application Programs</t>
+  </si>
+  <si>
+    <t>* Along with system programs, most operating systems are supplied with
+programs that are useful in solving common problems or performing common operations. Such application programs include Web browsers, word processors and text formatters, spreadsheets, database systems, compilers, plotting and statistical-analysis packages, and games.</t>
+  </si>
+  <si>
+    <t>OS Design and Implementation:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,6 +1774,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -544,7 +1805,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -554,6 +1815,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -837,8 +2101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A10"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1183,12 +2447,147 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="64.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="64.7109375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="285" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="285" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="345" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:A12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding some more files
</commit_message>
<xml_diff>
--- a/OperatingSystem/OperatingSystemConceptsHighLevelChart.xlsx
+++ b/OperatingSystem/OperatingSystemConceptsHighLevelChart.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
   <si>
     <t>Computer-System Operation</t>
   </si>
@@ -1749,6 +1749,105 @@
   </si>
   <si>
     <t>OS Design and Implementation:</t>
+  </si>
+  <si>
+    <t>Design Goals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Before design we have to define goals and specifications.
+* At the highest level, the design of the system will be affected by the choice of hardware and the type of system: batch, time sharing, single user, multiuser, distributed, real time, or general purpose.
+* Design requirements can, however, be divided into two basic groups:
+user goals and system goals.
+</t>
+  </si>
+  <si>
+    <t>Mechanisms and Policies</t>
+  </si>
+  <si>
+    <t>* One important principle is the separation of policy from mechanism. Mechanisms determine how to do something; policies determine what will be done. For example, the timer construct (see Section 1.5.2) is a mechanism for ensuring CPU protection, but deciding how long the timer is to be set for a particular user is a policy decision.</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>* Early operating systems were written in assembly language.
+* Nowdays most are written in a higher-level language such as C or an even higher-level language such as C++.
+* Actually, an operating system can be written in more than one language. The lowest levels of the kernel might be assembly language. Higher-level routines might be in C, and system programs might be in C or C++, in interpreted scripting languages like PERL or Python, or in shell scripts. In fact, a given Linux distribution probably includes programs written in all of those languages.
+* Master Control Program (MCP) OS written in Assembly language.
+* MULTICS OS is written in System Programming language PL/1.
+* The Linux and Windows operating system kernels are written mostly in C, although there are some small sections of assembly code for device drivers and for saving and restoring the state of registers.
+* MS-DOS was written in Intel 8088 assembly language. (It runs natively on Intel X86 family of CPUs)
+* The Linux operating system, in contrast, is written mostly in C and is available natively on a number of different CPUs, including Intel X86, Oracle SPARC, and IBMPowerPC.
+* major performance improvements in operating systems are more likely to be the result of better data structures and algorithms than of excellent assembly-language code.
+* In addition, although operating systems are large, only a small amount of the code is critical to high performance; the interrupt handler, I/O manager, memory manager, and CPU scheduler are probably the most critical routines.</t>
+  </si>
+  <si>
+    <t>OS Structure</t>
+  </si>
+  <si>
+    <t>Simple Structure</t>
+  </si>
+  <si>
+    <t>* MS-DOS is an example, it was written to provide most functionality in least space, so it was not carefully divided into modules.
+* Another example of limited structuring is the original UNIX operating
+system. Like MS-DOS, UNIX initially was limited by hardware functionality. It consists of two separable parts: the kernel and the system programs. Here The kernel provides the file system, CPU scheduling, memory management, and other operating-system functions through system calls.</t>
+  </si>
+  <si>
+    <t>Layered Approach</t>
+  </si>
+  <si>
+    <t>* Implementers have more freedom in changing the inner workings
+of the system and in creating modular operating systems. Under a topdown approach, the overall functionality and features are determined and are separated into components.
+*A system can be made modular in many ways. One method is the layered approach, in which the operating system is broken into a number of layers (levels). The bottom layer (layer 0) is the hardware; the highest (layer N) is the user interface.</t>
+  </si>
+  <si>
+    <t>Microkernels</t>
+  </si>
+  <si>
+    <t>* In the mid-1980s, researchers at Carnegie Mellon University developed an operating system called Mach that modularized the kernel using the microkernel approach. This method structures the operating system by removing all nonessential components fromthe kernel and implementing them as system and user-level programs.
+* There is little consensus regarding which services should remain in the
+kernel and which should be implemented in user space.
+* Microkernels provide minimal process and memory management, in addition to a communication facility i.e. Interprocess Communications, Memory Management and CPU Scheduling/Process management.
+* The main function of the microkernel is to provide communication between the client program and the various services that are also running in user space. Communication is provided through message passing,
+* One benefit of the microkernel approach is that it makes extending
+the operating system easier. All new services are added to user space and consequently do not require modification of the kernel. When the kernel does have to be modified, the changes tend to be fewer, because the microkernel is a smaller kernel. The resulting operating system is easier to port from one hardware design to another. The microkernel also provides more security and reliability, since most services are running as user—rather than kernel— processes. If a service fails, the rest of the operating system remains untouched.</t>
+  </si>
+  <si>
+    <t>Modules</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>* Perhaps the best current methodology for operating-system design involves using loadable kernel modules.
+* Here, the kernel has a set of core components and links in additional services via modules, either at boot time or during run time. This type of design is common in modern implementations of UNIX, such as Solaris, Linux, and Mac OS X, as well as Windows.
+* Linux also uses loadable kernel modules, primarily for supporting device drivers and file systems.</t>
+  </si>
+  <si>
+    <t>Hybrid Systems</t>
+  </si>
+  <si>
+    <t>* To address performance, security, and usability issues we need to combine different OS structures and resulting into Hybrid OS.
+* For example, both Linux and Solaris are monolithic, because having the operating system in a single address space provides very efficient performance. However, they are also modular, so that new functionality can be dynamically added to the kernel. Windows is largely monolithic as well (again primarily for performance reasons), but it retains some behavior typical of microkernel systems, including providing support for separate subsystems (known as operating-system personalities) that run as user-mode processes. Windows systems also provide support for dynamically loadable kernel modules.
+* Other exemples for Hybrid OS are Mac OS X, iOS and Android.</t>
+  </si>
+  <si>
+    <t>Failure Analysis</t>
+  </si>
+  <si>
+    <t>* A failure in the kernel is called a crash.When a crash occurs, error information is saved to a log file, and the memory state is saved to a crash dump.</t>
+  </si>
+  <si>
+    <t>Performance Tuning</t>
+  </si>
+  <si>
+    <t>* OS measures system behavior by producing "trace listings"  of system behavior. All interesting events are logged with their time and important
+parameters and are written to a file. Later, an analysis program can process the log file to determine system performance and to identify bottlenecks and inefficiencies.
+* Usageof "top" command in linux / unix like systems.
+* A new generation of kernel-enabled performance analysis tools has made significant improvements in how this goal can be achieved.</t>
+  </si>
+  <si>
+    <t>DTrace</t>
   </si>
 </sst>
 </file>
@@ -2101,8 +2200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2447,10 +2546,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="64.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2578,14 +2677,111 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>103</v>
       </c>
+      <c r="B15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="390" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="375" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>126</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A7:A12"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding Git related docs
</commit_message>
<xml_diff>
--- a/OperatingSystem/OperatingSystemConceptsHighLevelChart.xlsx
+++ b/OperatingSystem/OperatingSystemConceptsHighLevelChart.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VijayBI\GitHubCom\VBI\OperatingSystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBI\SCM\GitHubCom\VBI\OperatingSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20295" windowHeight="8445" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20292" windowHeight="8448" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -2105,16 +2105,16 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
-    <col min="2" max="2" width="52.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="56.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="39.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="52.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="56.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="1" t="s">
@@ -2138,7 +2138,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -2147,7 +2147,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -2156,7 +2156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>10</v>
@@ -2176,7 +2176,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
         <v>11</v>
@@ -2185,7 +2185,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="240" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
         <v>22</v>
@@ -2213,7 +2213,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="240" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -2237,13 +2237,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="144" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
         <v>31</v>
@@ -2252,13 +2252,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="375" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="375" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>36</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="1" t="s">
         <v>39</v>
@@ -2286,7 +2286,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="1" t="s">
         <v>41</v>
@@ -2295,7 +2295,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="1" t="s">
         <v>43</v>
@@ -2304,7 +2304,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>50</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="1" t="s">
         <v>47</v>
@@ -2324,7 +2324,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="405" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="360" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="1" t="s">
         <v>49</v>
@@ -2333,7 +2333,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="1" t="s">
         <v>52</v>
@@ -2342,7 +2342,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="1" t="s">
         <v>54</v>
@@ -2351,7 +2351,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="1" t="s">
         <v>56</v>
@@ -2360,7 +2360,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="1" t="s">
         <v>58</v>
@@ -2369,7 +2369,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="1" t="s">
         <v>60</v>
@@ -2378,7 +2378,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>62</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="300" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="1" t="s">
         <v>65</v>
@@ -2398,7 +2398,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="1" t="s">
         <v>68</v>
@@ -2407,7 +2407,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="1" t="s">
         <v>69</v>
@@ -2416,12 +2416,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="315" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
@@ -2450,20 +2450,20 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="64.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="64.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="64.7109375" style="2"/>
+    <col min="1" max="16384" width="64.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>75</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="285" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>76</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>79</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>81</v>
       </c>
@@ -2498,7 +2498,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>83</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>86</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="2" t="s">
         <v>89</v>
@@ -2526,7 +2526,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="285" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="216" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="2" t="s">
         <v>91</v>
@@ -2535,7 +2535,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="345" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="288" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
         <v>93</v>
@@ -2544,7 +2544,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="2" t="s">
         <v>95</v>
@@ -2553,7 +2553,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="2" t="s">
         <v>97</v>
@@ -2562,7 +2562,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>99</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>101</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>103</v>
       </c>

</xml_diff>

<commit_message>
adding new file also editing with comment
</commit_message>
<xml_diff>
--- a/OperatingSystem/OperatingSystemConceptsHighLevelChart.xlsx
+++ b/OperatingSystem/OperatingSystemConceptsHighLevelChart.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VijayBI\GitHubCom\VBI\OperatingSystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VBI\SCM\GitHubCom\VBI\OperatingSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20295" windowHeight="8445" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20292" windowHeight="8448" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
     <sheet name="OS Structures" sheetId="2" r:id="rId2"/>
+    <sheet name="ProcessManagement" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t>Computer-System Operation</t>
   </si>
@@ -1816,9 +1817,6 @@
     <t>Modules</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>* Perhaps the best current methodology for operating-system design involves using loadable kernel modules.
 * Here, the kernel has a set of core components and links in additional services via modules, either at boot time or during run time. This type of design is common in modern implementations of UNIX, such as Solaris, Linux, and Mac OS X, as well as Windows.
 * Linux also uses loadable kernel modules, primarily for supporting device drivers and file systems.</t>
@@ -1848,6 +1846,33 @@
   </si>
   <si>
     <t>DTrace</t>
+  </si>
+  <si>
+    <t>* Not gone though indepth.</t>
+  </si>
+  <si>
+    <t>OS Debugging</t>
+  </si>
+  <si>
+    <t>OS Generation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* The system must then be configured or generated for each specific computer site, a process sometimes known as system generation SYSGEN.
+* </t>
+  </si>
+  <si>
+    <t>System Boot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*  The procedure of starting a computer by loading the kernel is known as booting the system.
+* On most computer systems, a small piece of code known as the bootstrap program or bootstrap loader locates the kernel, loads it into main memory, and starts its execution.
+* </t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>* Read it again and again.</t>
   </si>
 </sst>
 </file>
@@ -2204,16 +2229,16 @@
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="46" style="1" customWidth="1"/>
-    <col min="2" max="2" width="52.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="56.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="39.7109375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="52.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="56.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -2227,7 +2252,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="1" t="s">
@@ -2237,7 +2262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="225" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -2246,7 +2271,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -2255,7 +2280,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -2266,7 +2291,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>10</v>
@@ -2275,7 +2300,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="374.4" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
         <v>11</v>
@@ -2284,7 +2309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -2292,7 +2317,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="240" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -2303,7 +2328,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
         <v>22</v>
@@ -2312,7 +2337,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="240" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -2320,7 +2345,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -2328,7 +2353,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -2336,13 +2361,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="180" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="144" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
         <v>31</v>
@@ -2351,13 +2376,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="375" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -2365,7 +2390,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="375" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>36</v>
       </c>
@@ -2376,7 +2401,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="1" t="s">
         <v>39</v>
@@ -2385,7 +2410,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="1" t="s">
         <v>41</v>
@@ -2394,7 +2419,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="1" t="s">
         <v>43</v>
@@ -2403,7 +2428,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>50</v>
       </c>
@@ -2414,7 +2439,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="1" t="s">
         <v>47</v>
@@ -2423,7 +2448,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="405" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="360" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="1" t="s">
         <v>49</v>
@@ -2432,7 +2457,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="1" t="s">
         <v>52</v>
@@ -2441,7 +2466,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="1" t="s">
         <v>54</v>
@@ -2450,7 +2475,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="1" t="s">
         <v>56</v>
@@ -2459,7 +2484,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="1" t="s">
         <v>58</v>
@@ -2468,7 +2493,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="1" t="s">
         <v>60</v>
@@ -2477,7 +2502,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>62</v>
       </c>
@@ -2488,7 +2513,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="300" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="1" t="s">
         <v>65</v>
@@ -2497,7 +2522,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="1" t="s">
         <v>68</v>
@@ -2506,7 +2531,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="144" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="1" t="s">
         <v>69</v>
@@ -2515,12 +2540,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="315" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
@@ -2546,23 +2571,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="64.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="64.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="64.7109375" style="2"/>
+    <col min="1" max="16384" width="64.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>75</v>
       </c>
@@ -2570,7 +2595,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="285" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>76</v>
       </c>
@@ -2581,7 +2606,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>79</v>
       </c>
@@ -2589,7 +2614,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>81</v>
       </c>
@@ -2597,7 +2622,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>83</v>
       </c>
@@ -2605,7 +2630,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="403.2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>86</v>
       </c>
@@ -2616,7 +2641,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="2" t="s">
         <v>89</v>
@@ -2625,7 +2650,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="285" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="216" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="2" t="s">
         <v>91</v>
@@ -2634,7 +2659,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="345" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="288" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
         <v>93</v>
@@ -2643,7 +2668,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="2" t="s">
         <v>95</v>
@@ -2652,7 +2677,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="2" t="s">
         <v>97</v>
@@ -2661,7 +2686,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>99</v>
       </c>
@@ -2669,7 +2694,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>101</v>
       </c>
@@ -2677,7 +2702,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>103</v>
       </c>
@@ -2688,7 +2713,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="2" t="s">
         <v>106</v>
@@ -2697,7 +2722,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="390" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="360" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="2" t="s">
         <v>108</v>
@@ -2706,7 +2731,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>110</v>
       </c>
@@ -2717,7 +2742,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="2" t="s">
         <v>113</v>
@@ -2726,7 +2751,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="375" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="2" t="s">
         <v>115</v>
@@ -2735,55 +2760,97 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C22" s="2" t="s">
+    </row>
+    <row r="23" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="2" t="s">
+    </row>
+    <row r="24" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>126</v>
       </c>
     </row>
+    <row r="26" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A23:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>